<commit_message>
Basic visualization of handles in web app
</commit_message>
<xml_diff>
--- a/GUI/used-cargo-plates/sw_src005_antiNelsonQuimby_cc6hb_h2handles.xlsx
+++ b/GUI/used-cargo-plates/sw_src005_antiNelsonQuimby_cc6hb_h2handles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/GUI/used-cargo-plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A75C4-327D-264E-B7FA-F0E227BD56E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{947A75C4-327D-264E-B7FA-F0E227BD56E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D008A8F-8B3B-460B-B0CC-9637933535CD}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1068" yWindow="1068" windowWidth="20214" windowHeight="12438" xr2:uid="{A6DA471F-3DB0-6A47-B698-4794F84DD224}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{A6DA471F-3DB0-6A47-B698-4794F84DD224}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="373">
   <si>
     <t>A</t>
   </si>
@@ -177,198 +177,6 @@
     <t>from P3299_SW</t>
   </si>
   <si>
-    <t>h2-pos1-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos2-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos3-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos4-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos5-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos6-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos7-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos8-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos9-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos10-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos11-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos12-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos13-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos14-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos15-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos16-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos17-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos18-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos19-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos20-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos21-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos22-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos23-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos24-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos25-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos26-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos27-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos28-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos29-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos30-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos31-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos32-antiNelson</t>
-  </si>
-  <si>
-    <t>h2-pos1-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos2-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos3-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos4-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos5-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos6-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos7-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos8-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos9-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos10-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos11-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos12-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos13-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos14-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos15-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos16-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos17-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos18-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos19-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos20-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos21-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos22-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos23-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos24-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos25-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos26-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos27-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos28-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos29-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos30-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos31-antiQuimby</t>
-  </si>
-  <si>
-    <t>h2-pos32-antiQuimby</t>
-  </si>
-  <si>
     <t>h2 handles anti-Nelson</t>
   </si>
   <si>
@@ -741,198 +549,6 @@
     <t>F08</t>
   </si>
   <si>
-    <t>loopctrl-h2-pos1-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos2-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos3-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos4-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos5-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos6-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos7-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos8-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos9-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos10-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos11-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos12-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos13-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos14-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos15-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos16-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos17-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos18-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos19-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos20-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos21-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos22-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos23-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos24-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos25-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos26-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos27-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos28-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos29-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos30-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos31-y0n9m4</t>
-  </si>
-  <si>
-    <t>loopctrl-h2-pos32-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos1-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos2-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos3-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos4-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos5-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos6-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos7-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos8-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos9-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos10-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos11-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos12-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos13-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos14-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos15-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos16-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos17-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos18-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos19-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos20-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos21-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos22-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos23-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos24-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos25-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos26-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos27-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos28-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos29-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos30-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos31-y0n9m4</t>
-  </si>
-  <si>
-    <t>mask-h2-pos32-y0n9m4</t>
-  </si>
-  <si>
     <t>mask-h2-y0n9m4</t>
   </si>
   <si>
@@ -1135,6 +751,402 @@
   </si>
   <si>
     <t>NAX</t>
+  </si>
+  <si>
+    <t>h2 handles anti_Nelson</t>
+  </si>
+  <si>
+    <t>h2 handles anti_Quimby</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos1_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos2_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos3_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos4_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos5_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos6_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos7_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos8_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos9_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos10_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos11_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos12_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos13_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos14_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos15_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos16_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos17_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos18_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos19_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos20_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos21_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos22_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos23_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos24_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos25_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos26_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos27_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos28_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos29_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos30_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos31_y0n9m4</t>
+  </si>
+  <si>
+    <t>loopctrl_h2_pos32_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos1_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos2_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos3_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos4_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos5_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos6_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos7_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos8_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos9_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos10_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos11_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos12_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos13_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos14_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos15_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos16_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos17_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos18_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos19_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos20_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos21_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos22_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos23_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos24_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos25_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos26_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos27_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos28_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos29_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos30_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos31_y0n9m4</t>
+  </si>
+  <si>
+    <t>mask_h2_pos32_y0n9m4</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos1</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos2</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos3</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos4</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos5</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos6</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos7</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos8</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos9</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos10</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos11</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos12</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos13</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos14</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos15</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos16</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos17</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos18</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos19</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos20</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos21</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos22</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos23</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos24</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos25</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos26</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos27</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos28</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos29</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos30</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos31</t>
+  </si>
+  <si>
+    <t>antiNelson_h2_pos32</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos1</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos2</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos3</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos4</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos5</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos6</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos7</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos8</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos9</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos10</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos11</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos12</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos13</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos14</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos15</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos16</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos17</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos18</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos19</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos20</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos21</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos22</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos23</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos24</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos25</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos26</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos27</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos28</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos29</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos30</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos31</t>
+  </si>
+  <si>
+    <t>antiQuimby_h2_pos32</t>
   </si>
 </sst>
 </file>
@@ -1357,6 +1369,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1658,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A330979C-A82F-6645-A34F-51C92A163A61}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="248" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="R2" zoomScale="168" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4:Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1750,79 +1766,79 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>309</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>310</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>311</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>312</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>53</v>
+        <v>313</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
+        <v>314</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>55</v>
+        <v>315</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>316</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>57</v>
+        <v>317</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>58</v>
+        <v>318</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>59</v>
+        <v>319</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>60</v>
+        <v>320</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>61</v>
+        <v>321</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>62</v>
+        <v>322</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>63</v>
+        <v>323</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>64</v>
+        <v>324</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>65</v>
+        <v>325</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>66</v>
+        <v>326</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>67</v>
+        <v>327</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>68</v>
+        <v>328</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>69</v>
+        <v>329</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>70</v>
+        <v>330</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>71</v>
+        <v>331</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>72</v>
+        <v>332</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>113</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.6">
@@ -1830,28 +1846,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>333</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>334</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>75</v>
+        <v>335</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>336</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>337</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>78</v>
+        <v>338</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>79</v>
+        <v>339</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>80</v>
+        <v>340</v>
       </c>
       <c r="Z3" s="18"/>
     </row>
@@ -1860,79 +1876,79 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>81</v>
+        <v>341</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>342</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>83</v>
+        <v>343</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>344</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>85</v>
+        <v>345</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>86</v>
+        <v>346</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>87</v>
+        <v>347</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>88</v>
+        <v>348</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>89</v>
+        <v>349</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>90</v>
+        <v>350</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>91</v>
+        <v>351</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>92</v>
+        <v>352</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>93</v>
+        <v>353</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>94</v>
+        <v>354</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>95</v>
+        <v>355</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>96</v>
+        <v>356</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>97</v>
+        <v>357</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>98</v>
+        <v>358</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>99</v>
+        <v>359</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>100</v>
+        <v>360</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>101</v>
+        <v>361</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>102</v>
+        <v>362</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>103</v>
+        <v>363</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>104</v>
+        <v>364</v>
       </c>
       <c r="Z4" s="19" t="s">
-        <v>114</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.6">
@@ -1940,28 +1956,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>105</v>
+        <v>365</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>366</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>107</v>
+        <v>367</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>108</v>
+        <v>368</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>109</v>
+        <v>369</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>110</v>
+        <v>370</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>111</v>
+        <v>371</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>112</v>
+        <v>372</v>
       </c>
       <c r="Z5" s="20"/>
     </row>
@@ -1970,60 +1986,60 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="Z6" s="21" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="AA6" t="s">
-        <v>367</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.6">
@@ -2031,52 +2047,52 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
@@ -2087,57 +2103,57 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="Z8" s="22" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.6">
@@ -2145,52 +2161,52 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
@@ -2255,8 +2271,8 @@
   </sheetPr>
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2347,79 +2363,79 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.6">
@@ -2427,28 +2443,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="Z3" s="17"/>
     </row>
@@ -2457,79 +2473,79 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.6">
@@ -2537,28 +2553,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>173</v>
+        <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>178</v>
+        <v>114</v>
       </c>
       <c r="Z5" s="20"/>
     </row>
@@ -2567,58 +2583,58 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>303</v>
+        <v>175</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>304</v>
+        <v>176</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>305</v>
+        <v>177</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>306</v>
+        <v>178</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>308</v>
+        <v>180</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>309</v>
+        <v>181</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>310</v>
+        <v>182</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>311</v>
+        <v>183</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>312</v>
+        <v>184</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>313</v>
+        <v>185</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>314</v>
+        <v>186</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>315</v>
+        <v>187</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>316</v>
+        <v>188</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>317</v>
+        <v>189</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>318</v>
+        <v>190</v>
       </c>
       <c r="Z6" s="21" t="s">
-        <v>302</v>
+        <v>174</v>
       </c>
       <c r="AA6" t="s">
-        <v>367</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.6">
@@ -2626,52 +2642,52 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>319</v>
+        <v>191</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>320</v>
+        <v>192</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>321</v>
+        <v>193</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>322</v>
+        <v>194</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>323</v>
+        <v>195</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>324</v>
+        <v>196</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>325</v>
+        <v>197</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>326</v>
+        <v>198</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>327</v>
+        <v>199</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>328</v>
+        <v>200</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>329</v>
+        <v>201</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>330</v>
+        <v>202</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>331</v>
+        <v>203</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>332</v>
+        <v>204</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>333</v>
+        <v>205</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>334</v>
+        <v>206</v>
       </c>
       <c r="Z7" s="21"/>
     </row>
@@ -2680,55 +2696,55 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>335</v>
+        <v>207</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>336</v>
+        <v>208</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>337</v>
+        <v>209</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>338</v>
+        <v>210</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>339</v>
+        <v>211</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>340</v>
+        <v>212</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>341</v>
+        <v>213</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>342</v>
+        <v>214</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>343</v>
+        <v>215</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>344</v>
+        <v>216</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>345</v>
+        <v>217</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>346</v>
+        <v>218</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>347</v>
+        <v>219</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>348</v>
+        <v>220</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>349</v>
+        <v>221</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>350</v>
+        <v>222</v>
       </c>
       <c r="Z8" s="22" t="s">
-        <v>301</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.6">
@@ -2736,52 +2752,52 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>351</v>
+        <v>223</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>352</v>
+        <v>224</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>353</v>
+        <v>225</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>354</v>
+        <v>226</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>355</v>
+        <v>227</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>356</v>
+        <v>228</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>357</v>
+        <v>229</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>358</v>
+        <v>230</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>359</v>
+        <v>231</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>360</v>
+        <v>232</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>361</v>
+        <v>233</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>362</v>
+        <v>234</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>363</v>
+        <v>235</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>364</v>
+        <v>236</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>366</v>
+        <v>238</v>
       </c>
       <c r="Z9" s="22"/>
     </row>
@@ -2976,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C4B945-413B-9446-9175-6E015252E944}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="107" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="P1" zoomScale="107" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3064,76 +3080,76 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.6">
@@ -3141,28 +3157,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.6">
@@ -3170,76 +3186,76 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.6">
@@ -3247,28 +3263,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.6">
@@ -3276,52 +3292,52 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.6">
@@ -3329,52 +3345,52 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.6">
@@ -3382,52 +3398,52 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.6">
@@ -3435,52 +3451,52 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.6">
@@ -3533,7 +3549,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3676,31 +3692,31 @@
         <v>0</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>179</v>
+        <v>115</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>182</v>
+        <v>118</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>183</v>
+        <v>119</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>186</v>
+        <v>122</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>40</v>
@@ -3712,31 +3728,31 @@
         <v>42</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>188</v>
+        <v>124</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="V4" s="15" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
       <c r="W4" s="15" t="s">
         <v>43</v>
@@ -3753,28 +3769,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
@@ -3798,76 +3814,76 @@
         <v>2</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>205</v>
+        <v>141</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>211</v>
+        <v>147</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>212</v>
+        <v>148</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>213</v>
+        <v>149</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>215</v>
+        <v>151</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>220</v>
+        <v>156</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>221</v>
+        <v>157</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="T6" s="15" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="U6" s="15" t="s">
-        <v>224</v>
+        <v>160</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>225</v>
+        <v>161</v>
       </c>
       <c r="W6" s="15" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="X6" s="15" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="Y6" s="15" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.6">
@@ -3875,28 +3891,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>231</v>
+        <v>167</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>232</v>
+        <v>168</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>234</v>
+        <v>170</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>236</v>
+        <v>172</v>
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>

</xml_diff>